<commit_message>
Interfaces definiert, neues Projekt
</commit_message>
<xml_diff>
--- a/doc/Funktionen.xlsx
+++ b/doc/Funktionen.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reimarklammer/Documents/sst_bankkomponenten/doc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\dev\sst_bankkomponenten\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17595" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Funktionsname</t>
   </si>
@@ -75,12 +75,15 @@
   </si>
   <si>
     <t>Umrechnungs faktor</t>
+  </si>
+  <si>
+    <t>Überweisen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -110,17 +113,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Stand." xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -389,19 +397,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -409,77 +417,83 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Implemented very simple Dataclasses.
</commit_message>
<xml_diff>
--- a/doc/Funktionen.xlsx
+++ b/doc/Funktionen.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17595" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17595" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="185">
   <si>
     <t>Funktionsname</t>
   </si>
@@ -78,6 +79,510 @@
   </si>
   <si>
     <t>Überweisen</t>
+  </si>
+  <si>
+    <t>AED</t>
+  </si>
+  <si>
+    <t>AFN</t>
+  </si>
+  <si>
+    <t>ALL</t>
+  </si>
+  <si>
+    <t>AMD</t>
+  </si>
+  <si>
+    <t>ANG</t>
+  </si>
+  <si>
+    <t>AOA</t>
+  </si>
+  <si>
+    <t>ARS</t>
+  </si>
+  <si>
+    <t>AUD</t>
+  </si>
+  <si>
+    <t>AWG</t>
+  </si>
+  <si>
+    <t>AZN</t>
+  </si>
+  <si>
+    <t>BAM</t>
+  </si>
+  <si>
+    <t>BBD</t>
+  </si>
+  <si>
+    <t>BDT</t>
+  </si>
+  <si>
+    <t>BGN</t>
+  </si>
+  <si>
+    <t>BHD</t>
+  </si>
+  <si>
+    <t>BIF</t>
+  </si>
+  <si>
+    <t>BMD</t>
+  </si>
+  <si>
+    <t>BND</t>
+  </si>
+  <si>
+    <t>BOB</t>
+  </si>
+  <si>
+    <t>BOV</t>
+  </si>
+  <si>
+    <t>BRL</t>
+  </si>
+  <si>
+    <t>BSD</t>
+  </si>
+  <si>
+    <t>BTN</t>
+  </si>
+  <si>
+    <t>BWP</t>
+  </si>
+  <si>
+    <t>BYN</t>
+  </si>
+  <si>
+    <t>BYR</t>
+  </si>
+  <si>
+    <t>BZD</t>
+  </si>
+  <si>
+    <t>CAD</t>
+  </si>
+  <si>
+    <t>CDF</t>
+  </si>
+  <si>
+    <t>CHE</t>
+  </si>
+  <si>
+    <t>CHF</t>
+  </si>
+  <si>
+    <t>CHW</t>
+  </si>
+  <si>
+    <t>CLF</t>
+  </si>
+  <si>
+    <t>CLP</t>
+  </si>
+  <si>
+    <t>CNY</t>
+  </si>
+  <si>
+    <t>COP</t>
+  </si>
+  <si>
+    <t>COU</t>
+  </si>
+  <si>
+    <t>CRC</t>
+  </si>
+  <si>
+    <t>CUC</t>
+  </si>
+  <si>
+    <t>CUP</t>
+  </si>
+  <si>
+    <t>CVE</t>
+  </si>
+  <si>
+    <t>CZK</t>
+  </si>
+  <si>
+    <t>DJF</t>
+  </si>
+  <si>
+    <t>DKK</t>
+  </si>
+  <si>
+    <t>DOP</t>
+  </si>
+  <si>
+    <t>DZD</t>
+  </si>
+  <si>
+    <t>EGP</t>
+  </si>
+  <si>
+    <t>ERN</t>
+  </si>
+  <si>
+    <t>ETB</t>
+  </si>
+  <si>
+    <t>EUR</t>
+  </si>
+  <si>
+    <t>FJD</t>
+  </si>
+  <si>
+    <t>FKP</t>
+  </si>
+  <si>
+    <t>GBP</t>
+  </si>
+  <si>
+    <t>GEL</t>
+  </si>
+  <si>
+    <t>GHS</t>
+  </si>
+  <si>
+    <t>GIP</t>
+  </si>
+  <si>
+    <t>GMD</t>
+  </si>
+  <si>
+    <t>GNF</t>
+  </si>
+  <si>
+    <t>GTQ</t>
+  </si>
+  <si>
+    <t>GYD</t>
+  </si>
+  <si>
+    <t>HKD</t>
+  </si>
+  <si>
+    <t>HNL</t>
+  </si>
+  <si>
+    <t>HRK</t>
+  </si>
+  <si>
+    <t>HTG</t>
+  </si>
+  <si>
+    <t>HUF</t>
+  </si>
+  <si>
+    <t>IDR</t>
+  </si>
+  <si>
+    <t>ILS</t>
+  </si>
+  <si>
+    <t>INR</t>
+  </si>
+  <si>
+    <t>IQD</t>
+  </si>
+  <si>
+    <t>IRR</t>
+  </si>
+  <si>
+    <t>ISK</t>
+  </si>
+  <si>
+    <t>JMD</t>
+  </si>
+  <si>
+    <t>JOD</t>
+  </si>
+  <si>
+    <t>JPY</t>
+  </si>
+  <si>
+    <t>KES</t>
+  </si>
+  <si>
+    <t>KGS</t>
+  </si>
+  <si>
+    <t>KHR</t>
+  </si>
+  <si>
+    <t>KMF</t>
+  </si>
+  <si>
+    <t>KPW</t>
+  </si>
+  <si>
+    <t>KRW</t>
+  </si>
+  <si>
+    <t>KWD</t>
+  </si>
+  <si>
+    <t>KYD</t>
+  </si>
+  <si>
+    <t>KZT</t>
+  </si>
+  <si>
+    <t>LAK</t>
+  </si>
+  <si>
+    <t>LBP</t>
+  </si>
+  <si>
+    <t>LKR</t>
+  </si>
+  <si>
+    <t>LRD</t>
+  </si>
+  <si>
+    <t>LSL</t>
+  </si>
+  <si>
+    <t>LYD</t>
+  </si>
+  <si>
+    <t>MAD</t>
+  </si>
+  <si>
+    <t>MDL</t>
+  </si>
+  <si>
+    <t>MGA</t>
+  </si>
+  <si>
+    <t>MKD</t>
+  </si>
+  <si>
+    <t>MMK</t>
+  </si>
+  <si>
+    <t>MNT</t>
+  </si>
+  <si>
+    <t>MOP</t>
+  </si>
+  <si>
+    <t>MRO</t>
+  </si>
+  <si>
+    <t>MUR</t>
+  </si>
+  <si>
+    <t>MVR</t>
+  </si>
+  <si>
+    <t>MWK</t>
+  </si>
+  <si>
+    <t>MXN</t>
+  </si>
+  <si>
+    <t>MXV</t>
+  </si>
+  <si>
+    <t>MYR</t>
+  </si>
+  <si>
+    <t>MZN</t>
+  </si>
+  <si>
+    <t>NAD</t>
+  </si>
+  <si>
+    <t>NGN</t>
+  </si>
+  <si>
+    <t>NIO</t>
+  </si>
+  <si>
+    <t>NOK</t>
+  </si>
+  <si>
+    <t>NPR</t>
+  </si>
+  <si>
+    <t>NZD</t>
+  </si>
+  <si>
+    <t>OMR</t>
+  </si>
+  <si>
+    <t>PAB</t>
+  </si>
+  <si>
+    <t>PEN</t>
+  </si>
+  <si>
+    <t>PGK</t>
+  </si>
+  <si>
+    <t>PHP</t>
+  </si>
+  <si>
+    <t>PKR</t>
+  </si>
+  <si>
+    <t>PLN</t>
+  </si>
+  <si>
+    <t>PYG</t>
+  </si>
+  <si>
+    <t>QAR</t>
+  </si>
+  <si>
+    <t>RON</t>
+  </si>
+  <si>
+    <t>RSD</t>
+  </si>
+  <si>
+    <t>RUB</t>
+  </si>
+  <si>
+    <t>RWF</t>
+  </si>
+  <si>
+    <t>SAR</t>
+  </si>
+  <si>
+    <t>SBD</t>
+  </si>
+  <si>
+    <t>SCR</t>
+  </si>
+  <si>
+    <t>SDG</t>
+  </si>
+  <si>
+    <t>SSP</t>
+  </si>
+  <si>
+    <t>SEK</t>
+  </si>
+  <si>
+    <t>SGD</t>
+  </si>
+  <si>
+    <t>SHP</t>
+  </si>
+  <si>
+    <t>SLL</t>
+  </si>
+  <si>
+    <t>SOS</t>
+  </si>
+  <si>
+    <t>SRD</t>
+  </si>
+  <si>
+    <t>STD</t>
+  </si>
+  <si>
+    <t>SVC</t>
+  </si>
+  <si>
+    <t>SYP</t>
+  </si>
+  <si>
+    <t>SZL</t>
+  </si>
+  <si>
+    <t>THB</t>
+  </si>
+  <si>
+    <t>TJS</t>
+  </si>
+  <si>
+    <t>TMT</t>
+  </si>
+  <si>
+    <t>TND</t>
+  </si>
+  <si>
+    <t>TOP</t>
+  </si>
+  <si>
+    <t>TRY</t>
+  </si>
+  <si>
+    <t>TTD</t>
+  </si>
+  <si>
+    <t>TWD</t>
+  </si>
+  <si>
+    <t>TZS</t>
+  </si>
+  <si>
+    <t>UAH</t>
+  </si>
+  <si>
+    <t>UGX</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>UYI</t>
+  </si>
+  <si>
+    <t>UYU</t>
+  </si>
+  <si>
+    <t>UZS</t>
+  </si>
+  <si>
+    <t>VEF</t>
+  </si>
+  <si>
+    <t>VND</t>
+  </si>
+  <si>
+    <t>VUV</t>
+  </si>
+  <si>
+    <t>WST</t>
+  </si>
+  <si>
+    <t>XAF</t>
+  </si>
+  <si>
+    <t>XCD</t>
+  </si>
+  <si>
+    <t>XOF</t>
+  </si>
+  <si>
+    <t>XPF</t>
+  </si>
+  <si>
+    <t>XSU</t>
+  </si>
+  <si>
+    <t>YER</t>
+  </si>
+  <si>
+    <t>ZAR</t>
+  </si>
+  <si>
+    <t>ZMW</t>
+  </si>
+  <si>
+    <t>ZWL</t>
+  </si>
+  <si>
+    <t>Währungscode</t>
+  </si>
+  <si>
+    <t>Integer Wert</t>
   </si>
 </sst>
 </file>
@@ -113,10 +618,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -399,7 +907,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
@@ -496,4 +1004,1353 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B167"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B30">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B33">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B34">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B36">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B37">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B38">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B39">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B40">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B41">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B42">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B43">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B44">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B45">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B46">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B47">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B48">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B49">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B50">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B51">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B52">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B53">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B54">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B55">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B56">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B57">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B58">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B59">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B60">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B61">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B62">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B63">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B64">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B65">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B66">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B67">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B68">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B69">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B70">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B71">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B72">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B73">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B74">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B75">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B76">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B77">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B78">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B79">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B80">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B81">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B82">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B83">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B84">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B85">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B86">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B87">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B88">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B89">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B90">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B91">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B92">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B93">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B94">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B95">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B96">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B97">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B98">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B99">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B100">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B101">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B102">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B103">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B104">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B105">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B106">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B107">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B108">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B109">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B110">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B111">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B112">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B113">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B114">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B115">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B116">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B117">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B118">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B119">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B120">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B121">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B122">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B123">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B124">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B125">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B126">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B127">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B128">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B129">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B130">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B131">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B132">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B133">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B134">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B135">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B136">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B137">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B138">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B139">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B140">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B141">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B142">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B143">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B144">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B145">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B146">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B147">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B148">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B149">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B150">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B151">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B152">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B153">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B154">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B155">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B156">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B157">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B158">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A159" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B159">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B160">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A161" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B161">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A162" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B162">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A163" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B163">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A164" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B164">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A165" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B165">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A166" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="B166">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A167" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B167">
+        <v>166</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Konto Sperren aus der API entfernt. Sinn?
</commit_message>
<xml_diff>
--- a/doc/Funktionen.xlsx
+++ b/doc/Funktionen.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="184">
   <si>
     <t>Funktionsname</t>
   </si>
@@ -49,9 +49,6 @@
   </si>
   <si>
     <t>Konto schließen</t>
-  </si>
-  <si>
-    <t>Konto sperren</t>
   </si>
   <si>
     <t>Konto Verfüger entfernen</t>
@@ -905,10 +902,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="A2:B2"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -952,32 +949,32 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -993,11 +990,6 @@
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1016,15 +1008,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B1" t="s">
         <v>183</v>
-      </c>
-      <c r="B1" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1032,7 +1024,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -1040,7 +1032,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -1048,7 +1040,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -1056,7 +1048,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -1064,7 +1056,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -1072,7 +1064,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -1080,7 +1072,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -1088,7 +1080,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -1096,7 +1088,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -1104,7 +1096,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -1112,7 +1104,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -1120,7 +1112,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -1128,7 +1120,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -1136,7 +1128,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -1144,7 +1136,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -1152,7 +1144,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -1160,7 +1152,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -1168,7 +1160,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -1176,7 +1168,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -1184,7 +1176,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B22">
         <v>21</v>
@@ -1192,7 +1184,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B23">
         <v>22</v>
@@ -1200,7 +1192,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B24">
         <v>23</v>
@@ -1208,7 +1200,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B25">
         <v>24</v>
@@ -1216,7 +1208,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B26">
         <v>25</v>
@@ -1224,7 +1216,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B27">
         <v>26</v>
@@ -1232,7 +1224,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B28">
         <v>27</v>
@@ -1240,7 +1232,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B29">
         <v>28</v>
@@ -1248,7 +1240,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B30">
         <v>29</v>
@@ -1256,7 +1248,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B31">
         <v>30</v>
@@ -1264,7 +1256,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B32">
         <v>31</v>
@@ -1272,7 +1264,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B33">
         <v>32</v>
@@ -1280,7 +1272,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B34">
         <v>33</v>
@@ -1288,7 +1280,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B35">
         <v>34</v>
@@ -1296,7 +1288,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B36">
         <v>35</v>
@@ -1304,7 +1296,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B37">
         <v>36</v>
@@ -1312,7 +1304,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B38">
         <v>37</v>
@@ -1320,7 +1312,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B39">
         <v>38</v>
@@ -1328,7 +1320,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B40">
         <v>39</v>
@@ -1336,7 +1328,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B41">
         <v>40</v>
@@ -1344,7 +1336,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B42">
         <v>41</v>
@@ -1352,7 +1344,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B43">
         <v>42</v>
@@ -1360,7 +1352,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B44">
         <v>43</v>
@@ -1368,7 +1360,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B45">
         <v>44</v>
@@ -1376,7 +1368,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B46">
         <v>45</v>
@@ -1384,7 +1376,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B47">
         <v>46</v>
@@ -1392,7 +1384,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B48">
         <v>47</v>
@@ -1400,7 +1392,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B49">
         <v>48</v>
@@ -1408,7 +1400,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B50">
         <v>49</v>
@@ -1416,7 +1408,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B51">
         <v>50</v>
@@ -1424,7 +1416,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B52">
         <v>51</v>
@@ -1432,7 +1424,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B53">
         <v>52</v>
@@ -1440,7 +1432,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B54">
         <v>53</v>
@@ -1448,7 +1440,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B55">
         <v>54</v>
@@ -1456,7 +1448,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B56">
         <v>55</v>
@@ -1464,7 +1456,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B57">
         <v>56</v>
@@ -1472,7 +1464,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B58">
         <v>57</v>
@@ -1480,7 +1472,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B59">
         <v>58</v>
@@ -1488,7 +1480,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B60">
         <v>59</v>
@@ -1496,7 +1488,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B61">
         <v>60</v>
@@ -1504,7 +1496,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B62">
         <v>61</v>
@@ -1512,7 +1504,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B63">
         <v>62</v>
@@ -1520,7 +1512,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B64">
         <v>63</v>
@@ -1528,7 +1520,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B65">
         <v>64</v>
@@ -1536,7 +1528,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B66">
         <v>65</v>
@@ -1544,7 +1536,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B67">
         <v>66</v>
@@ -1552,7 +1544,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B68">
         <v>67</v>
@@ -1560,7 +1552,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B69">
         <v>68</v>
@@ -1568,7 +1560,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B70">
         <v>69</v>
@@ -1576,7 +1568,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B71">
         <v>70</v>
@@ -1584,7 +1576,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B72">
         <v>71</v>
@@ -1592,7 +1584,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B73">
         <v>72</v>
@@ -1600,7 +1592,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B74">
         <v>73</v>
@@ -1608,7 +1600,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B75">
         <v>74</v>
@@ -1616,7 +1608,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B76">
         <v>75</v>
@@ -1624,7 +1616,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B77">
         <v>76</v>
@@ -1632,7 +1624,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B78">
         <v>77</v>
@@ -1640,7 +1632,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B79">
         <v>78</v>
@@ -1648,7 +1640,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B80">
         <v>79</v>
@@ -1656,7 +1648,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B81">
         <v>80</v>
@@ -1664,7 +1656,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B82">
         <v>81</v>
@@ -1672,7 +1664,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B83">
         <v>82</v>
@@ -1680,7 +1672,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B84">
         <v>83</v>
@@ -1688,7 +1680,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B85">
         <v>84</v>
@@ -1696,7 +1688,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B86">
         <v>85</v>
@@ -1704,7 +1696,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B87">
         <v>86</v>
@@ -1712,7 +1704,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B88">
         <v>87</v>
@@ -1720,7 +1712,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B89">
         <v>88</v>
@@ -1728,7 +1720,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B90">
         <v>89</v>
@@ -1736,7 +1728,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B91">
         <v>90</v>
@@ -1744,7 +1736,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B92">
         <v>91</v>
@@ -1752,7 +1744,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B93">
         <v>92</v>
@@ -1760,7 +1752,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B94">
         <v>93</v>
@@ -1768,7 +1760,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B95">
         <v>94</v>
@@ -1776,7 +1768,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B96">
         <v>95</v>
@@ -1784,7 +1776,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B97">
         <v>96</v>
@@ -1792,7 +1784,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B98">
         <v>97</v>
@@ -1800,7 +1792,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B99">
         <v>98</v>
@@ -1808,7 +1800,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B100">
         <v>99</v>
@@ -1816,7 +1808,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B101">
         <v>100</v>
@@ -1824,7 +1816,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B102">
         <v>101</v>
@@ -1832,7 +1824,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B103">
         <v>102</v>
@@ -1840,7 +1832,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B104">
         <v>103</v>
@@ -1848,7 +1840,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B105">
         <v>104</v>
@@ -1856,7 +1848,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B106">
         <v>105</v>
@@ -1864,7 +1856,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B107">
         <v>106</v>
@@ -1872,7 +1864,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B108">
         <v>107</v>
@@ -1880,7 +1872,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B109">
         <v>108</v>
@@ -1888,7 +1880,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B110">
         <v>109</v>
@@ -1896,7 +1888,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B111">
         <v>110</v>
@@ -1904,7 +1896,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B112">
         <v>111</v>
@@ -1912,7 +1904,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B113">
         <v>112</v>
@@ -1920,7 +1912,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B114">
         <v>113</v>
@@ -1928,7 +1920,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B115">
         <v>114</v>
@@ -1936,7 +1928,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B116">
         <v>115</v>
@@ -1944,7 +1936,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B117">
         <v>116</v>
@@ -1952,7 +1944,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B118">
         <v>117</v>
@@ -1960,7 +1952,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B119">
         <v>118</v>
@@ -1968,7 +1960,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B120">
         <v>119</v>
@@ -1976,7 +1968,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B121">
         <v>120</v>
@@ -1984,7 +1976,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B122">
         <v>121</v>
@@ -1992,7 +1984,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B123">
         <v>122</v>
@@ -2000,7 +1992,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B124">
         <v>123</v>
@@ -2008,7 +2000,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B125">
         <v>124</v>
@@ -2016,7 +2008,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B126">
         <v>125</v>
@@ -2024,7 +2016,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B127">
         <v>126</v>
@@ -2032,7 +2024,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B128">
         <v>127</v>
@@ -2040,7 +2032,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B129">
         <v>128</v>
@@ -2048,7 +2040,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B130">
         <v>129</v>
@@ -2056,7 +2048,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B131">
         <v>130</v>
@@ -2064,7 +2056,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B132">
         <v>131</v>
@@ -2072,7 +2064,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B133">
         <v>132</v>
@@ -2080,7 +2072,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B134">
         <v>133</v>
@@ -2088,7 +2080,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B135">
         <v>134</v>
@@ -2096,7 +2088,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B136">
         <v>135</v>
@@ -2104,7 +2096,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B137">
         <v>136</v>
@@ -2112,7 +2104,7 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B138">
         <v>137</v>
@@ -2120,7 +2112,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B139">
         <v>138</v>
@@ -2128,7 +2120,7 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B140">
         <v>139</v>
@@ -2136,7 +2128,7 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B141">
         <v>140</v>
@@ -2144,7 +2136,7 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B142">
         <v>141</v>
@@ -2152,7 +2144,7 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B143">
         <v>142</v>
@@ -2160,7 +2152,7 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B144">
         <v>143</v>
@@ -2168,7 +2160,7 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B145">
         <v>144</v>
@@ -2176,7 +2168,7 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B146">
         <v>145</v>
@@ -2184,7 +2176,7 @@
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B147">
         <v>146</v>
@@ -2192,7 +2184,7 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B148">
         <v>147</v>
@@ -2200,7 +2192,7 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B149">
         <v>148</v>
@@ -2208,7 +2200,7 @@
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B150">
         <v>149</v>
@@ -2216,7 +2208,7 @@
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B151">
         <v>150</v>
@@ -2224,7 +2216,7 @@
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B152">
         <v>151</v>
@@ -2232,7 +2224,7 @@
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B153">
         <v>152</v>
@@ -2240,7 +2232,7 @@
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B154">
         <v>153</v>
@@ -2248,7 +2240,7 @@
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B155">
         <v>154</v>
@@ -2256,7 +2248,7 @@
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B156">
         <v>155</v>
@@ -2264,7 +2256,7 @@
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B157">
         <v>156</v>
@@ -2272,7 +2264,7 @@
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B158">
         <v>157</v>
@@ -2280,7 +2272,7 @@
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B159">
         <v>158</v>
@@ -2288,7 +2280,7 @@
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B160">
         <v>159</v>
@@ -2296,7 +2288,7 @@
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B161">
         <v>160</v>
@@ -2304,7 +2296,7 @@
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B162">
         <v>161</v>
@@ -2312,7 +2304,7 @@
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B163">
         <v>162</v>
@@ -2320,7 +2312,7 @@
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B164">
         <v>163</v>
@@ -2328,7 +2320,7 @@
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B165">
         <v>164</v>
@@ -2336,7 +2328,7 @@
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B166">
         <v>165</v>
@@ -2344,7 +2336,7 @@
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B167">
         <v>166</v>

</xml_diff>